<commit_message>
implement init filtering logic
</commit_message>
<xml_diff>
--- a/storage/tests/sample.xlsx
+++ b/storage/tests/sample.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Win-7\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\html\power-parser\storage\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B85FC50-EEF1-4734-998D-34CB92B9C0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7344" windowHeight="1884"/>
+    <workbookView xWindow="6570" yWindow="1590" windowWidth="16395" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,95 +25,92 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
-  <si>
-    <t xml:space="preserve">رقم الصندوق </t>
-  </si>
-  <si>
-    <t>صندوق المعرض</t>
-  </si>
-  <si>
-    <t>العملة</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="25">
   <si>
     <t>SR</t>
   </si>
   <si>
-    <t>ريال سعودي</t>
-  </si>
-  <si>
-    <t>التاريخ</t>
-  </si>
-  <si>
-    <t>نوع المستند</t>
-  </si>
-  <si>
-    <t>رقم المستند</t>
-  </si>
-  <si>
-    <t>البيان</t>
-  </si>
-  <si>
-    <t>رقم المرجع</t>
-  </si>
-  <si>
-    <t>مدين</t>
-  </si>
-  <si>
-    <t>دائن</t>
-  </si>
-  <si>
-    <t>الرصيد الإفتتاحي</t>
-  </si>
-  <si>
     <t>21/09/2022</t>
   </si>
   <si>
-    <t>قيد يومية</t>
-  </si>
-  <si>
-    <t>فواتير مشتريات نقدية</t>
-  </si>
-  <si>
-    <t>سند صرف نقدي</t>
-  </si>
-  <si>
-    <t>فاتورة المبيعات نقد</t>
-  </si>
-  <si>
-    <t>مبيعات نقدية</t>
-  </si>
-  <si>
-    <t>فاتورة مردود المبيعات نقد</t>
-  </si>
-  <si>
-    <t>مردود مبيعات للفاتورة رقم    3625</t>
-  </si>
-  <si>
-    <t>مردودات نقدية</t>
-  </si>
-  <si>
-    <t>مردود مبيعات للفاتورة رقم    3599</t>
-  </si>
-  <si>
-    <t>مردود مبيعات للفاتورة رقم    3631</t>
-  </si>
-  <si>
-    <t>فاتورة المشتريات نقد</t>
-  </si>
-  <si>
-    <t>إجمالي العمليات</t>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Ref Number</t>
+  </si>
+  <si>
+    <t>Open Balance</t>
+  </si>
+  <si>
+    <t>Debit</t>
+  </si>
+  <si>
+    <t>Credit</t>
+  </si>
+  <si>
+    <t>Cashier Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Exhibit</t>
+  </si>
+  <si>
+    <t>Journal Entry</t>
+  </si>
+  <si>
+    <t>Payment Voucher</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Return for Invoice No. 3625</t>
+  </si>
+  <si>
+    <t>Return for Invoice No. 3599</t>
+  </si>
+  <si>
+    <t>Return for Invoice No. 3631</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Purchase</t>
+  </si>
+  <si>
+    <t>Cash purchase invoices</t>
+  </si>
+  <si>
+    <t>Saudi Riyal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -120,7 +118,7 @@
     <font>
       <sz val="17"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
@@ -448,70 +446,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.8984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="22.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="F3" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="22.5" x14ac:dyDescent="0.35">
+      <c r="D5" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="D5" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="F5" s="3">
         <v>9152.2512850000003</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -528,7 +528,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>23380.63</v>
@@ -536,10 +536,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>331</v>
@@ -550,10 +550,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>332</v>
@@ -564,10 +564,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>333</v>
@@ -578,16 +578,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>3627</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F11">
         <v>639.99699999999996</v>
@@ -595,16 +595,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C12">
         <v>3628</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F12">
         <v>45.011000000000003</v>
@@ -612,16 +612,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>3629</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F13">
         <v>460</v>
@@ -629,16 +629,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C14">
         <v>3630</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F14">
         <v>28.013999999999999</v>
@@ -646,16 +646,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <v>3631</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>227.0035</v>
@@ -663,16 +663,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>3632</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F16">
         <v>28.013999999999999</v>
@@ -680,16 +680,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>3633</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F17">
         <v>280.00200000000001</v>
@@ -697,16 +697,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C18">
         <v>3634</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F18">
         <v>104.99850000000001</v>
@@ -714,16 +714,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>3635</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F19">
         <v>220</v>
@@ -731,16 +731,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>3636</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F20">
         <v>140</v>
@@ -748,16 +748,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C21">
         <v>3637</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F21">
         <v>708.00900000000001</v>
@@ -765,16 +765,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C22">
         <v>3638</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F22">
         <v>1360.0129999999999</v>
@@ -782,16 +782,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C23">
         <v>3639</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F23">
         <v>152.07599999999999</v>
@@ -799,16 +799,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C24">
         <v>3640</v>
       </c>
       <c r="D24" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F24">
         <v>90.022000000000006</v>
@@ -816,16 +816,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C25">
         <v>3641</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F25">
         <v>460</v>
@@ -833,16 +833,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C26">
         <v>3642</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F26">
         <v>180.09</v>
@@ -850,16 +850,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C27">
         <v>3643</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F27">
         <v>432.33100000000002</v>
@@ -867,16 +867,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C28">
         <v>248</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G28">
         <v>269.99849999999998</v>
@@ -884,16 +884,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C29">
         <v>249</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G29">
         <v>100.004</v>
@@ -901,16 +901,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30">
         <v>250</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G30">
         <v>992.00149999999996</v>
@@ -918,16 +918,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C31">
         <v>251</v>
       </c>
       <c r="D31" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G31">
         <v>111.996</v>
@@ -935,10 +935,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32">
         <v>127</v>
@@ -949,10 +949,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>128</v>
@@ -963,10 +963,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F34">
         <v>28936.210999999999</v>
@@ -977,6 +977,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>